<commit_message>
Updated ID Repo Error message
</commit_message>
<xml_diff>
--- a/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint 10/Consolidated error messages V2.2.xlsx
+++ b/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint 10/Consolidated error messages V2.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\Requirements Detailing References\ID-Authentication\Sprint 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE13B25A-C373-42AD-8F1B-174D0627DD5A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0F4B3ED0-0381-4F99-9F9D-8E05B2D7A21C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDA" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="297">
   <si>
     <t>IDA-MLC-003</t>
   </si>
@@ -1056,6 +1056,9 @@
     <t>“Please register your &lt;Notification Channel&gt; and try again”</t>
   </si>
   <si>
+    <t>IDA-OTA-011</t>
+  </si>
+  <si>
     <t>"&lt;Notification Channel&gt; not configured for the country"</t>
   </si>
   <si>
@@ -1083,7 +1086,16 @@
     <t>“Device provider not registered with MOSIP”</t>
   </si>
   <si>
-    <t>IDA-OTA-001</t>
+    <t>IDA-MLC-017</t>
+  </si>
+  <si>
+    <t>Authorization Failed</t>
+  </si>
+  <si>
+    <t>Unauthorised roles accessing ID Repo Service</t>
+  </si>
+  <si>
+    <t>KER-IDR-021</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1210,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1213,31 +1225,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF5F5F5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEBECF0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1320,19 +1314,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1354,10 +1342,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1392,21 +1380,20 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1754,1245 +1741,1245 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="28.5" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="30" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="30"/>
-    <col min="3" max="3" width="44.42578125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="19.7109375" style="30" collapsed="1"/>
-    <col min="7" max="7" width="22.7109375" style="30" customWidth="1"/>
-    <col min="8" max="16384" width="19.7109375" style="30"/>
+    <col min="1" max="1" width="4.7109375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="25"/>
+    <col min="3" max="3" width="44.42578125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="19.7109375" style="25" collapsed="1"/>
+    <col min="7" max="7" width="22.7109375" style="25" customWidth="1"/>
+    <col min="8" max="16384" width="19.7109375" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" s="26" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" ht="110.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" ht="63" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" ht="157.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="H19" s="27"/>
+    </row>
+    <row r="20" spans="1:8" ht="63" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>23</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>24</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>25</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="D25" s="30"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>28</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>33</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>34</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>35</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>36</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="G30" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>37</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>38</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>39</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>40</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>41</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>42</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>43</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>44</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>46</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>47</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>48</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>49</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>50</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>51</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <v>52</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>53</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" s="27" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>54</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>55</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="1:11" ht="63" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>56</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="1:11" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>57</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>58</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>59</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>60</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>61</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>62</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>63</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13">
+        <v>64</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G57" s="28"/>
+    </row>
+    <row r="58" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>63</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59" spans="1:11" ht="94.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>64</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>65</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="19">
+        <v>66</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="D61" s="6"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G61" s="10"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="5"/>
+    </row>
+    <row r="62" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="20">
+        <v>22</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G62" s="21"/>
+    </row>
+    <row r="63" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="20">
+        <v>26</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="17"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="4">
+        <v>66</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="D64" s="10"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G64" s="24"/>
+      <c r="H64" s="22"/>
+    </row>
+    <row r="65" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="4">
+        <v>67</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="G65" s="4"/>
+      <c r="H65" s="23"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="6"/>
+    </row>
+    <row r="66" spans="1:12" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="19">
+        <v>67</v>
+      </c>
+      <c r="B66" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C66" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>282</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" s="31" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="110.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" ht="63" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" ht="157.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>17</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>18</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="H19" s="32"/>
-    </row>
-    <row r="20" spans="1:8" ht="63" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
-        <v>20</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>271</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>270</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
-        <v>21</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>273</v>
-      </c>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
-        <v>23</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
-        <v>24</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>289</v>
-      </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
-        <v>25</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>291</v>
-      </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
-        <v>28</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
-        <v>33</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
-        <v>34</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
-        <v>35</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:8" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
-        <v>36</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="G30" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
-        <v>37</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
-        <v>38</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
-        <v>39</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6">
-        <v>40</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
-        <v>41</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6">
-        <v>42</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
-        <v>43</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" ht="63" x14ac:dyDescent="0.2">
-      <c r="A38" s="6">
-        <v>44</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6">
-        <v>46</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="6">
-        <v>47</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="6">
-        <v>48</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="6">
-        <v>49</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6">
-        <v>50</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="6">
-        <v>51</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="6">
-        <v>52</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="6">
-        <v>53</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="G46" s="8"/>
-    </row>
-    <row r="47" spans="1:7" s="32" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="6">
-        <v>54</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="63" x14ac:dyDescent="0.2">
-      <c r="A48" s="6">
-        <v>55</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="1:11" ht="63" x14ac:dyDescent="0.2">
-      <c r="A49" s="6">
-        <v>56</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="G49" s="8"/>
-    </row>
-    <row r="50" spans="1:11" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="6">
-        <v>57</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="G50" s="8"/>
-    </row>
-    <row r="51" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
-        <v>58</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="6">
-        <v>59</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="G52" s="8"/>
-    </row>
-    <row r="53" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="6">
-        <v>60</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="G53" s="8"/>
-    </row>
-    <row r="54" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="6">
-        <v>61</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="G54" s="8"/>
-    </row>
-    <row r="55" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="6">
-        <v>62</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="G55" s="8"/>
-    </row>
-    <row r="56" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="6">
-        <v>63</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="G56" s="8"/>
-    </row>
-    <row r="57" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="15">
-        <v>64</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G57" s="33"/>
-    </row>
-    <row r="58" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="6">
-        <v>63</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="G58" s="8"/>
-    </row>
-    <row r="59" spans="1:11" ht="94.5" x14ac:dyDescent="0.2">
-      <c r="A59" s="6">
-        <v>64</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="G59" s="8"/>
-    </row>
-    <row r="60" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="6">
-        <v>65</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="G60" s="8"/>
-    </row>
-    <row r="61" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="21">
-        <v>66</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G61" s="12"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="7"/>
-    </row>
-    <row r="62" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="22">
-        <v>22</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F62" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G62" s="23"/>
-    </row>
-    <row r="63" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="22">
-        <v>26</v>
-      </c>
-      <c r="B63" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D63" s="19"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G63" s="8"/>
-    </row>
-    <row r="64" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="6">
-        <v>66</v>
-      </c>
-      <c r="B64" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="C64" s="27" t="s">
-        <v>278</v>
-      </c>
-      <c r="D64" s="27"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="29" t="s">
-        <v>275</v>
-      </c>
-      <c r="G64" s="26"/>
-      <c r="H64" s="24"/>
-    </row>
-    <row r="65" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="6">
-        <v>67</v>
-      </c>
-      <c r="B65" s="27" t="s">
-        <v>279</v>
-      </c>
-      <c r="C65" s="27" t="s">
-        <v>287</v>
-      </c>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="G65" s="6"/>
-      <c r="H65" s="25"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="8"/>
-    </row>
-    <row r="66" spans="1:12" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="21">
-        <v>67</v>
-      </c>
-      <c r="B66" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="C66" s="27" t="s">
+      <c r="D66" s="10"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="D66" s="27"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
     </row>
     <row r="68" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="35"/>
+      <c r="C68" s="29"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F66" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -3006,8 +2993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3030,289 +3017,298 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="32" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="32" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="32" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="32" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="32" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="32" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="32" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="32" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="32" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="32" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="32" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="32" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="32" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="32" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="32" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="32" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="32" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="32" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="32" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="32" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>296</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated error messages for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint 10/Consolidated error messages V2.2.xlsx
+++ b/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint 10/Consolidated error messages V2.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\Requirements Detailing References\ID-Authentication\Sprint 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0F4B3ED0-0381-4F99-9F9D-8E05B2D7A21C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F9E71639-CDC6-4552-8F42-3D016B405A2E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDA" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="296">
   <si>
     <t>IDA-MLC-003</t>
   </si>
@@ -354,9 +354,6 @@
     <t xml:space="preserve">Missing biometric data in MOSIP database </t>
   </si>
   <si>
-    <t>“Missing biometric data in MOSIP database for the given UIN/Virtual ID.”</t>
-  </si>
-  <si>
     <t>IDA-BIA-011</t>
   </si>
   <si>
@@ -375,9 +372,6 @@
     <t>Individual’s data not available</t>
   </si>
   <si>
-    <t>“Individual’s data currently not available”</t>
-  </si>
-  <si>
     <t>Invalid reqPfr</t>
   </si>
   <si>
@@ -747,15 +741,9 @@
     <t>File(s) not found in DFS</t>
   </si>
   <si>
-    <t>“Demographic data  &lt;demo attribute&gt;  in  &lt;Language Code&gt; did not match”</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please re-enter your  &lt;demo attribute&gt;  in &lt;Language Code&gt; </t>
   </si>
   <si>
-    <t>name, Full Address, Address line Items, Gender Mismatch in any language</t>
-  </si>
-  <si>
     <t>“Demographic data – &lt;demo attribute&gt; did not match.”</t>
   </si>
   <si>
@@ -817,9 +805,6 @@
   </si>
   <si>
     <t>IDA-OTA-009</t>
-  </si>
-  <si>
-    <t>IDA-EKA-001</t>
   </si>
   <si>
     <t>IDA-DEA-003</t>
@@ -1097,12 +1082,66 @@
   <si>
     <t>KER-IDR-021</t>
   </si>
+  <si>
+    <t>“Biometric data &lt;Biometric Attribute&gt; not available in database.”</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">“Demographic data  &lt;demo attribute&gt;  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>in  &lt;Language Code&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (if applicable) did not match”</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"Demographic data  &lt;Demographic Attribute&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in &lt;Language Code&gt; (if applicable) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> not available in database.””</t>
+    </r>
+  </si>
+  <si>
+    <t>name, Full Address, Address line Items, Gender, Phone,e-mail,DOB,DOB Type, and age Mismatch in any language</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1209,8 +1248,15 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1232,6 +1278,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1314,7 +1366,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1393,6 +1445,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1741,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="28.5" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1750,7 +1808,7 @@
     <col min="1" max="1" width="4.7109375" style="25" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" style="25"/>
     <col min="3" max="3" width="44.42578125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" style="25" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="19.7109375" style="25" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="19.7109375" style="25" collapsed="1"/>
     <col min="7" max="7" width="22.7109375" style="25" customWidth="1"/>
@@ -1777,7 +1835,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1791,7 +1849,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>5</v>
@@ -1812,7 +1870,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>1</v>
@@ -1833,7 +1891,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>18</v>
@@ -1854,7 +1912,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>22</v>
@@ -1869,19 +1927,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G6" s="6"/>
     </row>
@@ -1896,7 +1954,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>27</v>
@@ -1990,7 +2048,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -2004,15 +2062,15 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G13" s="6"/>
     </row>
@@ -2021,35 +2079,35 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="126" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>211</v>
+      <c r="B15" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>293</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="F15" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F15" s="33" t="s">
         <v>48</v>
       </c>
       <c r="G15" s="6"/>
@@ -2065,10 +2123,10 @@
         <v>51</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>53</v>
@@ -2099,15 +2157,15 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G18" s="6"/>
     </row>
@@ -2127,7 +2185,7 @@
         <v>57</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H19" s="27"/>
     </row>
@@ -2135,20 +2193,20 @@
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>214</v>
+      <c r="B20" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>210</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>236</v>
+      <c r="F20" s="34" t="s">
+        <v>231</v>
       </c>
       <c r="G20" s="6"/>
     </row>
@@ -2157,13 +2215,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>52</v>
@@ -2187,10 +2245,10 @@
         <v>66</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="G22" s="6"/>
     </row>
@@ -2202,7 +2260,7 @@
         <v>71</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -2216,15 +2274,15 @@
         <v>24</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="G24" s="6"/>
     </row>
@@ -2233,10 +2291,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="10"/>
@@ -2249,19 +2307,19 @@
       <c r="A26" s="4">
         <v>28</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>80</v>
+      <c r="C26" s="33" t="s">
+        <v>292</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="F26" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="F26" s="33" t="s">
         <v>72</v>
       </c>
       <c r="G26" s="6"/>
@@ -2271,13 +2329,13 @@
         <v>33</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>58</v>
@@ -2292,10 +2350,10 @@
         <v>34</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -2304,20 +2362,20 @@
       </c>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>35</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>87</v>
+      <c r="B29" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>294</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="5" t="s">
-        <v>235</v>
+      <c r="F29" s="33" t="s">
+        <v>231</v>
       </c>
       <c r="G29" s="6"/>
     </row>
@@ -2326,15 +2384,15 @@
         <v>36</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G30" s="12">
         <v>2</v>
@@ -2345,15 +2403,15 @@
         <v>37</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>225</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G31" s="6"/>
     </row>
@@ -2362,15 +2420,15 @@
         <v>38</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G32" s="6"/>
     </row>
@@ -2379,15 +2437,15 @@
         <v>39</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G33" s="6"/>
     </row>
@@ -2396,15 +2454,15 @@
         <v>40</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G34" s="6"/>
     </row>
@@ -2413,15 +2471,15 @@
         <v>41</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G35" s="6"/>
     </row>
@@ -2445,15 +2503,15 @@
         <v>43</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G37" s="6"/>
     </row>
@@ -2462,15 +2520,15 @@
         <v>44</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G38" s="6"/>
     </row>
@@ -2479,10 +2537,10 @@
         <v>46</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -2496,19 +2554,19 @@
         <v>47</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G40" s="6"/>
     </row>
@@ -2517,15 +2575,15 @@
         <v>48</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G41" s="6"/>
     </row>
@@ -2534,15 +2592,15 @@
         <v>49</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G42" s="6"/>
     </row>
@@ -2551,15 +2609,15 @@
         <v>50</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G43" s="6"/>
     </row>
@@ -2568,15 +2626,15 @@
         <v>51</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="14"/>
       <c r="F44" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G44" s="6"/>
     </row>
@@ -2585,19 +2643,19 @@
         <v>52</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>60</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G45" s="6"/>
     </row>
@@ -2606,17 +2664,17 @@
         <v>53</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G46" s="6"/>
     </row>
@@ -2625,20 +2683,20 @@
         <v>54</v>
       </c>
       <c r="B47" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>182</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>184</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="63" x14ac:dyDescent="0.2">
@@ -2646,15 +2704,15 @@
         <v>55</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G48" s="6"/>
     </row>
@@ -2663,15 +2721,15 @@
         <v>56</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G49" s="6"/>
     </row>
@@ -2680,15 +2738,15 @@
         <v>57</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G50" s="6"/>
     </row>
@@ -2697,15 +2755,15 @@
         <v>58</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G51" s="6"/>
     </row>
@@ -2714,15 +2772,15 @@
         <v>59</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G52" s="6"/>
     </row>
@@ -2731,15 +2789,15 @@
         <v>60</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G53" s="6"/>
     </row>
@@ -2748,15 +2806,15 @@
         <v>61</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G54" s="6"/>
     </row>
@@ -2765,15 +2823,15 @@
         <v>62</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G55" s="6"/>
     </row>
@@ -2782,15 +2840,15 @@
         <v>63</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G56" s="6"/>
     </row>
@@ -2799,15 +2857,15 @@
         <v>64</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G57" s="28"/>
     </row>
@@ -2816,15 +2874,15 @@
         <v>63</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G58" s="6"/>
     </row>
@@ -2833,15 +2891,15 @@
         <v>64</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G59" s="6"/>
     </row>
@@ -2850,15 +2908,15 @@
         <v>65</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G60" s="6"/>
     </row>
@@ -2867,15 +2925,15 @@
         <v>66</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G61" s="10"/>
       <c r="H61" s="6"/>
@@ -2891,7 +2949,7 @@
         <v>68</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D62" s="16" t="s">
         <v>69</v>
@@ -2917,7 +2975,7 @@
       <c r="D63" s="17"/>
       <c r="E63" s="15"/>
       <c r="F63" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G63" s="6"/>
     </row>
@@ -2926,15 +2984,15 @@
         <v>66</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64" s="14"/>
       <c r="F64" s="14" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G64" s="24"/>
       <c r="H64" s="22"/>
@@ -2944,15 +3002,15 @@
         <v>67</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
       <c r="F65" s="14" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="23"/>
@@ -2965,15 +3023,15 @@
         <v>67</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D66" s="10"/>
       <c r="E66" s="31"/>
       <c r="F66" s="10" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
@@ -2993,7 +3051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -3004,7 +3062,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
@@ -3021,13 +3079,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>128</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3035,13 +3093,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>131</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3049,13 +3107,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>134</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3063,13 +3121,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3077,13 +3135,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3091,13 +3149,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="32" t="s">
         <v>141</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3105,13 +3163,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>144</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3119,13 +3177,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="32" t="s">
         <v>147</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3133,13 +3191,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="32" t="s">
         <v>150</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3147,13 +3205,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3161,13 +3219,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="32" t="s">
         <v>153</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3175,13 +3233,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="32" t="s">
         <v>156</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3189,13 +3247,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="32" t="s">
         <v>159</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3203,13 +3261,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>162</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3217,13 +3275,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3231,13 +3289,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3245,13 +3303,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3259,13 +3317,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3273,13 +3331,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3287,13 +3345,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3301,13 +3359,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>